<commit_message>
updated with Sunday Gospel Canticles in OT
</commit_message>
<xml_diff>
--- a/psalm_metadata.xlsx
+++ b/psalm_metadata.xlsx
@@ -3475,18 +3475,18 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="27.85"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="9.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="21.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="21.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="8" style="3" width="9.13"/>
   </cols>
   <sheetData>
@@ -7860,9 +7860,9 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15"/>
@@ -9693,7 +9693,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.14"/>
@@ -9820,7 +9820,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.7"/>
@@ -12335,7 +12335,7 @@
       <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.86"/>

</xml_diff>